<commit_message>
Mon Dec 30 01:04:44 PM EST 2024
</commit_message>
<xml_diff>
--- a/iron_oxo_DDCASPT2/MAE_stacked.xlsx
+++ b/iron_oxo_DDCASPT2/MAE_stacked.xlsx
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1993983565843923</v>
+        <v>0.1964723900037332</v>
       </c>
       <c r="C2" t="n">
-        <v>4.097128095504559</v>
+        <v>4.95718404746367</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2912932630241646</v>
+        <v>0.2061449038404378</v>
       </c>
       <c r="C3" t="n">
-        <v>6.207020359206581</v>
+        <v>5.272444997864113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tue Dec 31 11:27:48 AM EST 2024
</commit_message>
<xml_diff>
--- a/iron_oxo_DDCASPT2/MAE_stacked.xlsx
+++ b/iron_oxo_DDCASPT2/MAE_stacked.xlsx
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1964723900037332</v>
+        <v>0.04562342498972654</v>
       </c>
       <c r="C2" t="n">
-        <v>4.95718404746367</v>
+        <v>1.152029883462799</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2061449038404378</v>
+        <v>0.06693906232308582</v>
       </c>
       <c r="C3" t="n">
-        <v>5.272444997864113</v>
+        <v>2.992764033751882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>